<commit_message>
Month two week one sat update
</commit_message>
<xml_diff>
--- a/Bootcamp/data/SFO_CreAcc.xlsx
+++ b/Bootcamp/data/SFO_CreAcc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14475" windowHeight="2400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14475" windowHeight="1935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>